<commit_message>
graph now allows you to click on nodes
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8922AF6-AC13-4C28-8762-5AAFDF81E079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8561B2AD-AB5A-4539-9028-9A8611F98D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="4080" windowWidth="29040" windowHeight="16440" xr2:uid="{5B11EEC1-C2D8-4C1E-A2F9-57042B1AA602}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="75">
   <si>
     <t>CI_Type</t>
   </si>
@@ -233,18 +233,6 @@
     <t xml:space="preserve"> A business intelligence tool used to design and generate interactive and formatted reports from a wide range of data sources, often used with MS SQL Server for reporting purposes.</t>
   </si>
   <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>X2</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>Y2</t>
-  </si>
-  <si>
     <t>Applications</t>
   </si>
   <si>
@@ -267,6 +255,12 @@
   </si>
   <si>
     <t>root</t>
+  </si>
+  <si>
+    <t>Windows Server</t>
+  </si>
+  <si>
+    <t>VMWare</t>
   </si>
 </sst>
 </file>
@@ -674,11 +668,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28AE7C4D-C8B9-4B8F-A7A2-DA0855C731E6}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:A9"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -718,13 +712,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -741,13 +735,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
@@ -756,7 +750,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>17</v>
@@ -764,13 +758,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>5</v>
@@ -779,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>17</v>
@@ -787,13 +781,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>5</v>
@@ -810,13 +804,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>5</v>
@@ -833,13 +827,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>5</v>
@@ -848,7 +842,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>17</v>
@@ -856,13 +850,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
@@ -871,7 +865,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>17</v>
@@ -879,13 +873,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>5</v>
@@ -894,7 +888,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>17</v>
@@ -1098,7 +1092,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>20</v>
@@ -1121,7 +1115,7 @@
         <v>5</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>20</v>
@@ -1144,7 +1138,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>20</v>
@@ -1167,7 +1161,7 @@
         <v>5</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>20</v>
@@ -1190,7 +1184,7 @@
         <v>5</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>20</v>
@@ -1213,7 +1207,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>20</v>
@@ -1236,7 +1230,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>20</v>
@@ -1259,7 +1253,7 @@
         <v>5</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>20</v>
@@ -1282,7 +1276,7 @@
         <v>5</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>20</v>
@@ -1305,7 +1299,7 @@
         <v>5</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>20</v>
@@ -1328,7 +1322,7 @@
         <v>5</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>20</v>
@@ -1351,7 +1345,7 @@
         <v>5</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>20</v>
@@ -1374,7 +1368,7 @@
         <v>5</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>20</v>
@@ -1397,7 +1391,7 @@
         <v>5</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>20</v>
@@ -1420,7 +1414,7 @@
         <v>5</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>20</v>
@@ -1443,7 +1437,7 @@
         <v>5</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>20</v>
@@ -1466,7 +1460,7 @@
         <v>5</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>20</v>
@@ -1489,7 +1483,7 @@
         <v>5</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>20</v>
@@ -1512,7 +1506,7 @@
         <v>5</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>20</v>
@@ -1535,7 +1529,7 @@
         <v>5</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>20</v>
@@ -1558,7 +1552,7 @@
         <v>5</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>20</v>
@@ -1581,7 +1575,7 @@
         <v>5</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>20</v>
@@ -1604,7 +1598,7 @@
         <v>5</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>20</v>
@@ -1627,7 +1621,7 @@
         <v>5</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>20</v>
@@ -1650,7 +1644,7 @@
         <v>5</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>20</v>
@@ -1673,7 +1667,7 @@
         <v>5</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>20</v>
@@ -1799,10 +1793,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>52</v>
@@ -1822,10 +1816,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>52</v>
@@ -1845,19 +1839,19 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>20</v>
@@ -1868,24 +1862,576 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C52" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C52" s="5" t="s">
         <v>52</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G52" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A53" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A54" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A55" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A56" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A57" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A58" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A59" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A60" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A61" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A62" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A63" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A64" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A65" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A66" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A67" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A68" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A69" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A70" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A71" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A72" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A73" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A74" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A75" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E75" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A76" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G76" s="3" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
serach and clicking node now results in the same graph output
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8561B2AD-AB5A-4539-9028-9A8611F98D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7487027-92EA-4BB3-892C-208B743962C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="4080" windowWidth="29040" windowHeight="16440" xr2:uid="{5B11EEC1-C2D8-4C1E-A2F9-57042B1AA602}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="79">
   <si>
     <t>CI_Type</t>
   </si>
@@ -236,9 +236,6 @@
     <t>Applications</t>
   </si>
   <si>
-    <t>Description..</t>
-  </si>
-  <si>
     <t xml:space="preserve">Automated Licensing Information System (ALIS) </t>
   </si>
   <si>
@@ -261,6 +258,21 @@
   </si>
   <si>
     <t>VMWare</t>
+  </si>
+  <si>
+    <t>An application is software designed to perform specific tasks or solve problems for users. It can run on platforms like desktops, mobile devices, web browsers, or cloud environments, offering interfaces for interacting with hardware, data, or services.</t>
+  </si>
+  <si>
+    <t>UPMIS relies on this person.</t>
+  </si>
+  <si>
+    <t>Computer or software system that provides resources, data, services, or programs to other computers, called clients, over a network to UPMIS.</t>
+  </si>
+  <si>
+    <t>Windows Server is a server operating system developed by Microsoft, designed to manage enterprise-level networks, applications, and services. It provides features for hosting websites, managing files, running applications, and offering centralized network control.…</t>
+  </si>
+  <si>
+    <t>A leading software company that specializes in virtualization and cloud computing technologies. Its products allow organizations to run multiple operating systems and applications on a single physical server or computer by creating virtual machines (VMs), each functioning as an independent system.</t>
   </si>
 </sst>
 </file>
@@ -671,8 +683,8 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -710,15 +722,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -733,15 +745,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
@@ -750,21 +762,21 @@
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>5</v>
@@ -773,21 +785,21 @@
         <v>3</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>5</v>
@@ -802,15 +814,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>5</v>
@@ -825,15 +837,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>5</v>
@@ -842,21 +854,21 @@
         <v>3</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
@@ -865,21 +877,21 @@
         <v>3</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>5</v>
@@ -888,7 +900,7 @@
         <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>17</v>
@@ -994,7 +1006,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>5</v>
@@ -1017,7 +1029,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>5</v>
@@ -1040,7 +1052,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>5</v>
@@ -1063,7 +1075,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>5</v>
@@ -1078,7 +1090,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -1086,13 +1098,13 @@
         <v>27</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>20</v>
@@ -1101,7 +1113,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>21</v>
       </c>
@@ -1109,13 +1121,13 @@
         <v>28</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>20</v>
@@ -1124,7 +1136,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>21</v>
       </c>
@@ -1132,13 +1144,13 @@
         <v>6</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>20</v>
@@ -1147,7 +1159,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -1155,13 +1167,13 @@
         <v>29</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>20</v>
@@ -1170,7 +1182,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1178,13 +1190,13 @@
         <v>30</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>20</v>
@@ -1193,7 +1205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1201,13 +1213,13 @@
         <v>31</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>20</v>
@@ -1216,7 +1228,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>21</v>
       </c>
@@ -1224,13 +1236,13 @@
         <v>32</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>20</v>
@@ -1239,7 +1251,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
@@ -1247,13 +1259,13 @@
         <v>33</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>20</v>
@@ -1262,7 +1274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
@@ -1270,13 +1282,13 @@
         <v>34</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>20</v>
@@ -1285,7 +1297,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
@@ -1293,13 +1305,13 @@
         <v>35</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>20</v>
@@ -1308,7 +1320,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
@@ -1316,13 +1328,13 @@
         <v>36</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>20</v>
@@ -1331,7 +1343,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>21</v>
       </c>
@@ -1339,13 +1351,13 @@
         <v>37</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>20</v>
@@ -1354,7 +1366,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>21</v>
       </c>
@@ -1362,13 +1374,13 @@
         <v>38</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>20</v>
@@ -1377,7 +1389,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>21</v>
       </c>
@@ -1385,13 +1397,13 @@
         <v>39</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>20</v>
@@ -1400,7 +1412,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>21</v>
       </c>
@@ -1408,13 +1420,13 @@
         <v>40</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>20</v>
@@ -1423,7 +1435,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>21</v>
       </c>
@@ -1431,13 +1443,13 @@
         <v>41</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>20</v>
@@ -1446,7 +1458,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>21</v>
       </c>
@@ -1454,13 +1466,13 @@
         <v>42</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>20</v>
@@ -1469,7 +1481,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>21</v>
       </c>
@@ -1477,13 +1489,13 @@
         <v>43</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>20</v>
@@ -1492,7 +1504,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>21</v>
       </c>
@@ -1500,13 +1512,13 @@
         <v>44</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>20</v>
@@ -1515,7 +1527,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>21</v>
       </c>
@@ -1523,13 +1535,13 @@
         <v>45</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>20</v>
@@ -1538,7 +1550,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>21</v>
       </c>
@@ -1546,13 +1558,13 @@
         <v>46</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>20</v>
@@ -1561,7 +1573,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>21</v>
       </c>
@@ -1569,13 +1581,13 @@
         <v>47</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>20</v>
@@ -1584,7 +1596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>21</v>
       </c>
@@ -1592,13 +1604,13 @@
         <v>48</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>20</v>
@@ -1607,7 +1619,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>21</v>
       </c>
@@ -1615,13 +1627,13 @@
         <v>49</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>20</v>
@@ -1630,7 +1642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>21</v>
       </c>
@@ -1638,13 +1650,13 @@
         <v>50</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>20</v>
@@ -1653,7 +1665,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>21</v>
       </c>
@@ -1661,13 +1673,13 @@
         <v>51</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>20</v>
@@ -1791,15 +1803,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" ht="128.25" x14ac:dyDescent="0.45">
       <c r="A49" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>5</v>
@@ -1814,15 +1826,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" ht="142.5" x14ac:dyDescent="0.45">
       <c r="A50" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>5</v>
@@ -1851,7 +1863,7 @@
         <v>5</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>20</v>
@@ -1874,7 +1886,7 @@
         <v>5</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>20</v>
@@ -1897,7 +1909,7 @@
         <v>5</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>20</v>
@@ -1920,7 +1932,7 @@
         <v>5</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>20</v>
@@ -1943,7 +1955,7 @@
         <v>5</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>20</v>
@@ -1966,7 +1978,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>20</v>
@@ -1989,7 +2001,7 @@
         <v>5</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>20</v>
@@ -2012,7 +2024,7 @@
         <v>5</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>20</v>
@@ -2035,7 +2047,7 @@
         <v>5</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>20</v>
@@ -2058,7 +2070,7 @@
         <v>5</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>20</v>
@@ -2081,7 +2093,7 @@
         <v>5</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>20</v>
@@ -2104,7 +2116,7 @@
         <v>5</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>20</v>
@@ -2127,7 +2139,7 @@
         <v>5</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>20</v>
@@ -2150,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>20</v>
@@ -2173,7 +2185,7 @@
         <v>5</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>20</v>
@@ -2196,7 +2208,7 @@
         <v>5</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>20</v>
@@ -2219,7 +2231,7 @@
         <v>5</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>20</v>
@@ -2242,7 +2254,7 @@
         <v>5</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>20</v>
@@ -2265,7 +2277,7 @@
         <v>5</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>20</v>
@@ -2288,7 +2300,7 @@
         <v>5</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>20</v>
@@ -2311,7 +2323,7 @@
         <v>5</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>20</v>
@@ -2334,7 +2346,7 @@
         <v>5</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>20</v>
@@ -2357,7 +2369,7 @@
         <v>5</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>20</v>
@@ -2380,7 +2392,7 @@
         <v>5</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>20</v>
@@ -2403,7 +2415,7 @@
         <v>5</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>20</v>
@@ -2426,7 +2438,7 @@
         <v>5</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
fixed issue where dependencies was showing parent node.
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7487027-92EA-4BB3-892C-208B743962C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52521C4-8023-43FE-9EAB-D5FAD911FD58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="4080" windowWidth="29040" windowHeight="16440" xr2:uid="{5B11EEC1-C2D8-4C1E-A2F9-57042B1AA602}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="86">
   <si>
     <t>CI_Type</t>
   </si>
@@ -236,24 +236,6 @@
     <t>Applications</t>
   </si>
   <si>
-    <t xml:space="preserve">Automated Licensing Information System (ALIS) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Electronic Management of Investigative &amp; Licensing Information (EMILI) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Coverage and Compliance Automated System (CCAS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Legal Service of Process (LSOP)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	Automated Investigative Management System (AIMS)</t>
-  </si>
-  <si>
-    <t>root</t>
-  </si>
-  <si>
     <t>Windows Server</t>
   </si>
   <si>
@@ -273,6 +255,45 @@
   </si>
   <si>
     <t>A leading software company that specializes in virtualization and cloud computing technologies. Its products allow organizations to run multiple operating systems and applications on a single physical server or computer by creating virtual machines (VMs), each functioning as an independent system.</t>
+  </si>
+  <si>
+    <t>Root</t>
+  </si>
+  <si>
+    <t>ALIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	EMILI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	CCAS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	LSOP</t>
+  </si>
+  <si>
+    <t>Automated Licensing Information System</t>
+  </si>
+  <si>
+    <t>Electronic Management of Investigative &amp; Licensing Information</t>
+  </si>
+  <si>
+    <t>Coverage and Compliance Automated System</t>
+  </si>
+  <si>
+    <t>Legal Service of Process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	AIMS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automated Investigative Management System </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florida State Fire College Electronic Information Database </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Florida Accounting Information Resource </t>
   </si>
 </sst>
 </file>
@@ -683,8 +704,8 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -724,13 +745,13 @@
     </row>
     <row r="2" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -747,13 +768,13 @@
     </row>
     <row r="3" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
@@ -762,21 +783,21 @@
         <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>5</v>
@@ -785,21 +806,21 @@
         <v>3</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>5</v>
@@ -811,18 +832,18 @@
         <v>53</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>5</v>
@@ -834,18 +855,18 @@
         <v>54</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>5</v>
@@ -854,21 +875,21 @@
         <v>3</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>
@@ -877,21 +898,21 @@
         <v>3</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>5</v>
@@ -900,10 +921,10 @@
         <v>3</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>17</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
@@ -1006,7 +1027,7 @@
         <v>23</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>5</v>
@@ -1029,7 +1050,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>5</v>
@@ -1052,7 +1073,7 @@
         <v>25</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>5</v>
@@ -1075,7 +1096,7 @@
         <v>26</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>5</v>
@@ -1098,13 +1119,13 @@
         <v>27</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>20</v>
@@ -1121,13 +1142,13 @@
         <v>28</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>20</v>
@@ -1144,13 +1165,13 @@
         <v>6</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>20</v>
@@ -1167,13 +1188,13 @@
         <v>29</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>20</v>
@@ -1190,13 +1211,13 @@
         <v>30</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>20</v>
@@ -1213,13 +1234,13 @@
         <v>31</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>20</v>
@@ -1236,13 +1257,13 @@
         <v>32</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>20</v>
@@ -1259,13 +1280,13 @@
         <v>33</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>20</v>
@@ -1282,13 +1303,13 @@
         <v>34</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>20</v>
@@ -1305,13 +1326,13 @@
         <v>35</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>20</v>
@@ -1328,13 +1349,13 @@
         <v>36</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>20</v>
@@ -1351,13 +1372,13 @@
         <v>37</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>20</v>
@@ -1374,13 +1395,13 @@
         <v>38</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>20</v>
@@ -1397,13 +1418,13 @@
         <v>39</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>20</v>
@@ -1420,13 +1441,13 @@
         <v>40</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>20</v>
@@ -1443,13 +1464,13 @@
         <v>41</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>20</v>
@@ -1466,13 +1487,13 @@
         <v>42</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>20</v>
@@ -1489,13 +1510,13 @@
         <v>43</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>20</v>
@@ -1512,13 +1533,13 @@
         <v>44</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>20</v>
@@ -1535,13 +1556,13 @@
         <v>45</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>20</v>
@@ -1558,13 +1579,13 @@
         <v>46</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>20</v>
@@ -1581,13 +1602,13 @@
         <v>47</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>20</v>
@@ -1604,13 +1625,13 @@
         <v>48</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>20</v>
@@ -1627,13 +1648,13 @@
         <v>49</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>20</v>
@@ -1650,13 +1671,13 @@
         <v>50</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>20</v>
@@ -1673,13 +1694,13 @@
         <v>51</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>20</v>
@@ -1808,10 +1829,10 @@
         <v>18</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>5</v>
@@ -1831,10 +1852,10 @@
         <v>18</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>5</v>
@@ -1863,7 +1884,7 @@
         <v>5</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F51" s="3" t="s">
         <v>20</v>
@@ -1886,7 +1907,7 @@
         <v>5</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>20</v>
@@ -1909,7 +1930,7 @@
         <v>5</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>20</v>
@@ -1932,7 +1953,7 @@
         <v>5</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>20</v>
@@ -1955,7 +1976,7 @@
         <v>5</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>20</v>
@@ -1978,7 +1999,7 @@
         <v>5</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F56" s="3" t="s">
         <v>20</v>
@@ -2001,7 +2022,7 @@
         <v>5</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>20</v>
@@ -2024,7 +2045,7 @@
         <v>5</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>20</v>
@@ -2047,7 +2068,7 @@
         <v>5</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>20</v>
@@ -2070,7 +2091,7 @@
         <v>5</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>20</v>
@@ -2093,7 +2114,7 @@
         <v>5</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F61" s="3" t="s">
         <v>20</v>
@@ -2116,7 +2137,7 @@
         <v>5</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>20</v>
@@ -2139,7 +2160,7 @@
         <v>5</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>20</v>
@@ -2162,7 +2183,7 @@
         <v>5</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>20</v>
@@ -2185,7 +2206,7 @@
         <v>5</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>20</v>
@@ -2208,7 +2229,7 @@
         <v>5</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>20</v>
@@ -2231,7 +2252,7 @@
         <v>5</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>20</v>
@@ -2254,7 +2275,7 @@
         <v>5</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>20</v>
@@ -2277,7 +2298,7 @@
         <v>5</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>20</v>
@@ -2300,7 +2321,7 @@
         <v>5</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F70" s="3" t="s">
         <v>20</v>
@@ -2323,7 +2344,7 @@
         <v>5</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>20</v>
@@ -2346,7 +2367,7 @@
         <v>5</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>20</v>
@@ -2369,7 +2390,7 @@
         <v>5</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>20</v>
@@ -2392,7 +2413,7 @@
         <v>5</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F74" s="3" t="s">
         <v>20</v>
@@ -2415,7 +2436,7 @@
         <v>5</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>20</v>
@@ -2438,7 +2459,7 @@
         <v>5</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
slide feature good for now...
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF81A5B-DAD4-44FF-95ED-BEB27D429D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74D66B5-9D94-4507-AD64-32DDDB3BC0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="4080" windowWidth="29040" windowHeight="16440" xr2:uid="{5B11EEC1-C2D8-4C1E-A2F9-57042B1AA602}"/>
   </bookViews>
@@ -270,7 +270,7 @@
 RFQ paid Monthly and purchased on behalf of Rob Williams in support of Application Development and Support - Consumer Protection</t>
   </si>
   <si>
-    <t>Staff Aug</t>
+    <t>Peoples</t>
   </si>
 </sst>
 </file>
@@ -684,8 +684,8 @@
   <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -763,7 +763,7 @@
         <v>10</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>45</v>
@@ -838,7 +838,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" ht="171" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -846,7 +846,7 @@
         <v>18</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>5</v>
@@ -861,7 +861,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="114" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" ht="199.5" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
@@ -869,7 +869,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
added eventlistener for for enter key on search
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56F6B5BD-2EC7-4F60-B141-4D89A5625320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E6832E-F03B-4C6C-9C3A-55B9C0824D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="705" windowWidth="14400" windowHeight="8723" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,21 +68,6 @@
     <t>Depends On</t>
   </si>
   <si>
-    <t>App1</t>
-  </si>
-  <si>
-    <t>App2</t>
-  </si>
-  <si>
-    <t>App3</t>
-  </si>
-  <si>
-    <t>App4</t>
-  </si>
-  <si>
-    <t>App5</t>
-  </si>
-  <si>
     <t>People</t>
   </si>
   <si>
@@ -180,6 +165,21 @@
   </si>
   <si>
     <t>Parent Description…</t>
+  </si>
+  <si>
+    <t>App 1</t>
+  </si>
+  <si>
+    <t>App 2</t>
+  </si>
+  <si>
+    <t>App 3</t>
+  </si>
+  <si>
+    <t>App 4</t>
+  </si>
+  <si>
+    <t>App 5</t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -617,7 +617,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -628,7 +628,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>9</v>
@@ -637,10 +637,10 @@
         <v>8</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -651,7 +651,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>9</v>
@@ -660,10 +660,10 @@
         <v>8</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
@@ -674,7 +674,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>9</v>
@@ -683,10 +683,10 @@
         <v>8</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
@@ -697,7 +697,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>9</v>
@@ -706,10 +706,10 @@
         <v>8</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
@@ -720,7 +720,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>9</v>
@@ -729,10 +729,10 @@
         <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
@@ -743,19 +743,19 @@
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
@@ -766,19 +766,19 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
@@ -789,19 +789,19 @@
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
@@ -812,19 +812,19 @@
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
@@ -835,19 +835,19 @@
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="G11" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
@@ -858,19 +858,19 @@
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
@@ -881,19 +881,19 @@
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
@@ -904,19 +904,19 @@
         <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
@@ -927,19 +927,19 @@
         <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
@@ -950,19 +950,19 @@
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
@@ -973,19 +973,19 @@
         <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
@@ -996,19 +996,19 @@
         <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
@@ -1019,19 +1019,19 @@
         <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
@@ -1042,19 +1042,19 @@
         <v>7</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
@@ -1065,19 +1065,19 @@
         <v>7</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>32</v>
-      </c>
       <c r="G21" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.45">
@@ -1088,19 +1088,19 @@
         <v>7</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.45">
@@ -1111,19 +1111,19 @@
         <v>7</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.45">
@@ -1134,19 +1134,19 @@
         <v>7</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.45">
@@ -1157,19 +1157,19 @@
         <v>7</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.45">
@@ -1180,19 +1180,19 @@
         <v>7</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="G26" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.45">
@@ -1203,19 +1203,19 @@
         <v>7</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.45">
@@ -1226,19 +1226,19 @@
         <v>7</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.45">
@@ -1249,19 +1249,19 @@
         <v>7</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.45">
@@ -1272,19 +1272,19 @@
         <v>7</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.45">
@@ -1295,19 +1295,19 @@
         <v>7</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>9</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>44</v>
-      </c>
       <c r="G31" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed tooltip and updated graph behavior (more padding around nodes)
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E6832E-F03B-4C6C-9C3A-55B9C0824D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6773EE7D-229C-464E-B76D-E05BD1EC53DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="48">
   <si>
     <t>CI_Type</t>
   </si>
@@ -580,15 +580,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="9.06640625" style="3"/>
+    <col min="1" max="1" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" style="3"/>
     <col min="3" max="3" width="16.46484375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.9296875" style="3" bestFit="1" customWidth="1"/>
@@ -1310,6 +1311,121 @@
         <v>41</v>
       </c>
     </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A32" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
nodes will not move unless being dragged
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE73681F-AEF6-4DB9-886F-6D27F07DA5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ACA356-6666-400F-AEFA-E595CBF6D564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
+    <workbookView xWindow="-28950" yWindow="3390" windowWidth="28800" windowHeight="12225" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -582,15 +582,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.06640625" style="3"/>
-    <col min="3" max="3" width="16.46484375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.46484375" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.9296875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="3" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
keep nodes fixed when moving other nodes, click on node in right container and becomes active node
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ACA356-6666-400F-AEFA-E595CBF6D564}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F972EA0-40B7-4ED7-A1F3-C88C1486FBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28950" yWindow="3390" windowWidth="28800" windowHeight="12225" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
+    <workbookView xWindow="-19500" yWindow="1290" windowWidth="19470" windowHeight="21300" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="48">
   <si>
     <t>CI_Type</t>
   </si>
@@ -580,21 +580,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" style="3"/>
+    <col min="1" max="1" width="10.46484375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="16.46484375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.46484375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.9296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.46484375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.9296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16" style="3" customWidth="1"/>
+    <col min="7" max="7" width="21.59765625" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
@@ -1426,6 +1426,121 @@
         <v>41</v>
       </c>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
right container is alphabetical order
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F972EA0-40B7-4ED7-A1F3-C88C1486FBE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D1D7EC-A1C2-4035-8A63-73A2C6F8335D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19500" yWindow="1290" windowWidth="19470" windowHeight="21300" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="48">
   <si>
     <t>CI_Type</t>
   </si>
@@ -176,10 +176,10 @@
     <t>App 3</t>
   </si>
   <si>
+    <t>App 5</t>
+  </si>
+  <si>
     <t>App 4</t>
-  </si>
-  <si>
-    <t>App 5</t>
   </si>
 </sst>
 </file>
@@ -580,21 +580,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.46484375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.06640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="16.46484375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10.46484375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.9296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16" style="3" customWidth="1"/>
-    <col min="7" max="7" width="21.59765625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="14.06640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.796875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.59765625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="21.46484375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="26" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
@@ -707,7 +707,7 @@
         <v>8</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>41</v>
@@ -730,7 +730,7 @@
         <v>8</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>41</v>
@@ -1334,7 +1334,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>8</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>8</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>8</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>8</v>
       </c>
@@ -1426,120 +1426,31 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="G37" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A39" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A41" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>41</v>
-      </c>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="H42" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
adjusted search input field
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1026F69-55A3-4F05-945E-ADA8BBE8BA73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC77EBAA-6041-42C5-9354-BA6EF6CE796F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="48">
   <si>
     <t>CI_Type</t>
   </si>
@@ -180,36 +180,6 @@
   </si>
   <si>
     <t>App 4</t>
-  </si>
-  <si>
-    <t>Dependency Description...</t>
-  </si>
-  <si>
-    <t>APerson 4</t>
-  </si>
-  <si>
-    <t>BTech 1</t>
-  </si>
-  <si>
-    <t>CLocation 3</t>
-  </si>
-  <si>
-    <t>APO 1</t>
-  </si>
-  <si>
-    <t>XData 4</t>
-  </si>
-  <si>
-    <t>HPerson 5</t>
-  </si>
-  <si>
-    <t>OTech 4</t>
-  </si>
-  <si>
-    <t>ZLocation 2</t>
-  </si>
-  <si>
-    <t>SPerson 2</t>
   </si>
 </sst>
 </file>
@@ -610,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1364,7 +1334,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>8</v>
       </c>
@@ -1387,7 +1357,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>8</v>
       </c>
@@ -1410,7 +1380,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>8</v>
       </c>
@@ -1433,7 +1403,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>8</v>
       </c>
@@ -1456,7 +1426,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>8</v>
       </c>
@@ -1479,857 +1449,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A42" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H42" s="2"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A43" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A44" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A45" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A46" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A47" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A48" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B48" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A49" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B49" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F49" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A50" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G50" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A51" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F51" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A52" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E52" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F52" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A53" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A54" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A55" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F55" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A56" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A57" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G57" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A58" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A59" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A60" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A61" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A62" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A63" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A64" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A65" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A66" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F66" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A67" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A68" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A69" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A70" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A71" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F71" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G71" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A72" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B72" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C72" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F72" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A73" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B73" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A74" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B74" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F74" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>48</v>
-      </c>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
hover box for description
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6546FC73-FB4E-46CA-BD7A-46C86FA29BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0380DE-CDE3-45D6-A283-46DAC36F1696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="48">
   <si>
     <t>CI_Type</t>
   </si>
@@ -187,12 +187,6 @@
   </si>
   <si>
     <t>Organization</t>
-  </si>
-  <si>
-    <t>Dependency_Type_Descrip</t>
-  </si>
-  <si>
-    <t>Business description…</t>
   </si>
 </sst>
 </file>
@@ -596,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:H36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -609,13 +603,12 @@
     <col min="3" max="3" width="21.796875" style="3" customWidth="1"/>
     <col min="4" max="4" width="15" style="3" customWidth="1"/>
     <col min="5" max="5" width="21.59765625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23" style="3" customWidth="1"/>
-    <col min="7" max="7" width="21.46484375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="26" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.06640625" style="3"/>
+    <col min="6" max="6" width="21.46484375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="26" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="9.06640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,16 +625,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>47</v>
       </c>
@@ -658,16 +648,13 @@
         <v>7</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G2" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>47</v>
       </c>
@@ -684,16 +671,13 @@
         <v>7</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H3" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G3" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -710,16 +694,13 @@
         <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G4" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>47</v>
       </c>
@@ -736,16 +717,13 @@
         <v>7</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G5" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>47</v>
       </c>
@@ -762,16 +740,13 @@
         <v>7</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H6" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G6" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>47</v>
       </c>
@@ -788,16 +763,13 @@
         <v>9</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G7" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>47</v>
       </c>
@@ -814,16 +786,13 @@
         <v>9</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>47</v>
       </c>
@@ -840,16 +809,13 @@
         <v>9</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G9" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>47</v>
       </c>
@@ -866,16 +832,13 @@
         <v>9</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H10" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G10" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>47</v>
       </c>
@@ -892,16 +855,13 @@
         <v>9</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G11" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>47</v>
       </c>
@@ -918,16 +878,13 @@
         <v>15</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G12" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>47</v>
       </c>
@@ -944,16 +901,13 @@
         <v>15</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G13" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>47</v>
       </c>
@@ -970,16 +924,13 @@
         <v>15</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G14" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>47</v>
       </c>
@@ -996,16 +947,13 @@
         <v>15</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G15" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>47</v>
       </c>
@@ -1022,16 +970,13 @@
         <v>15</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G16" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
@@ -1048,16 +993,13 @@
         <v>21</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G17" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>47</v>
       </c>
@@ -1074,16 +1016,13 @@
         <v>21</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G18" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
@@ -1100,16 +1039,13 @@
         <v>21</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G19" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>47</v>
       </c>
@@ -1126,16 +1062,13 @@
         <v>21</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G20" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>47</v>
       </c>
@@ -1152,16 +1085,13 @@
         <v>21</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G21" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>47</v>
       </c>
@@ -1178,16 +1108,13 @@
         <v>27</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G22" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>47</v>
       </c>
@@ -1204,16 +1131,13 @@
         <v>27</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H23" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G23" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>47</v>
       </c>
@@ -1230,16 +1154,13 @@
         <v>27</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G24" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>47</v>
       </c>
@@ -1256,16 +1177,13 @@
         <v>27</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H25" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G25" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>47</v>
       </c>
@@ -1282,16 +1200,13 @@
         <v>27</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H26" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G26" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>47</v>
       </c>
@@ -1308,16 +1223,13 @@
         <v>33</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G27" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>47</v>
       </c>
@@ -1334,16 +1246,13 @@
         <v>33</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G28" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H28" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G28" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>47</v>
       </c>
@@ -1360,16 +1269,13 @@
         <v>33</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G29" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H29" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G29" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>47</v>
       </c>
@@ -1386,16 +1292,13 @@
         <v>33</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H30" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G30" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>47</v>
       </c>
@@ -1412,16 +1315,13 @@
         <v>33</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H31" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G31" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>47</v>
       </c>
@@ -1438,16 +1338,13 @@
         <v>33</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H32" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G32" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1464,16 +1361,13 @@
         <v>27</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G33" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H33" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G33" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1490,16 +1384,13 @@
         <v>9</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H34" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G34" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1516,16 +1407,13 @@
         <v>21</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G35" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H35" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="G35" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -1542,16 +1430,13 @@
         <v>15</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G36" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H36" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="G36" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new node type
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0380DE-CDE3-45D6-A283-46DAC36F1696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C839E439-85D9-4219-97E2-7D1011376683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
+    <workbookView xWindow="38280" yWindow="4080" windowWidth="29040" windowHeight="16440" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="57">
   <si>
     <t>CI_Type</t>
   </si>
@@ -187,6 +187,33 @@
   </si>
   <si>
     <t>Organization</t>
+  </si>
+  <si>
+    <t>Location 20</t>
+  </si>
+  <si>
+    <t>PO 20</t>
+  </si>
+  <si>
+    <t>Person 20</t>
+  </si>
+  <si>
+    <t>Data 20</t>
+  </si>
+  <si>
+    <t>Tech 20</t>
+  </si>
+  <si>
+    <t>People 1</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Server 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Server </t>
   </si>
 </sst>
 </file>
@@ -590,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1326,7 +1353,7 @@
         <v>47</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>46</v>
@@ -1335,10 +1362,10 @@
         <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>46</v>
@@ -1358,10 +1385,10 @@
         <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>46</v>
@@ -1381,10 +1408,10 @@
         <v>8</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>46</v>
@@ -1404,10 +1431,10 @@
         <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>46</v>
@@ -1427,17 +1454,132 @@
         <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A42" s="2"/>
+      <c r="F37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A43" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
implementing new backend structure to current set up
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0936338-0A50-4DB9-98D6-ACF6AC132657}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90693FA1-7DC8-45DE-AE1C-E49B9F0F49F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="4080" windowWidth="29040" windowHeight="16440" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
+    <workbookView xWindow="38295" yWindow="4200" windowWidth="14610" windowHeight="16305" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="53">
   <si>
     <t>CI_Type</t>
   </si>
@@ -197,9 +197,6 @@
   <si>
     <t xml:space="preserve">Business description...
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">People </t>
   </si>
 </sst>
 </file>
@@ -618,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.45"/>
@@ -1464,29 +1461,6 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="21" x14ac:dyDescent="0.45">
-      <c r="A37" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
everything works but group toggles
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90693FA1-7DC8-45DE-AE1C-E49B9F0F49F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAA0FB17-47B4-44B0-BC06-C9BEFDDA2773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38295" yWindow="4200" windowWidth="14610" windowHeight="16305" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
+    <workbookView xWindow="38280" yWindow="4080" windowWidth="29040" windowHeight="16440" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="54">
   <si>
     <t>CI_Type</t>
   </si>
@@ -197,6 +197,9 @@
   <si>
     <t xml:space="preserve">Business description...
 </t>
+  </si>
+  <si>
+    <t>App 20</t>
   </si>
 </sst>
 </file>
@@ -615,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.45"/>
@@ -1461,6 +1464,29 @@
         <v>52</v>
       </c>
     </row>
+    <row r="37" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions headings="1" gridLines="1"/>

</xml_diff>

<commit_message>
added fonts, collapse left and right pane
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B819610B-9698-45D1-8D12-11848817166E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358FA640-42BC-4F78-9FC6-7BD135EFCA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
+    <workbookView xWindow="38280" yWindow="4080" windowWidth="29040" windowHeight="16440" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="61">
   <si>
     <t>CI_Type</t>
   </si>
@@ -216,6 +216,13 @@
   </si>
   <si>
     <t xml:space="preserve">Business description...
+Attribute 1: Value
+Attribute 2: Value
+Attribute 3: Value
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Business description…HELLO
 Attribute 1: Value
 Attribute 2: Value
 Attribute 3: Value
@@ -679,7 +686,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -699,10 +706,10 @@
         <v>40</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
@@ -722,10 +729,10 @@
         <v>41</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
@@ -745,10 +752,10 @@
         <v>42</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -768,10 +775,10 @@
         <v>44</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>45</v>
       </c>
@@ -791,10 +798,10 @@
         <v>43</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
@@ -814,10 +821,10 @@
         <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
@@ -837,10 +844,10 @@
         <v>11</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>45</v>
       </c>
@@ -860,10 +867,10 @@
         <v>12</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
@@ -883,10 +890,10 @@
         <v>13</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
@@ -906,10 +913,10 @@
         <v>14</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
@@ -929,10 +936,10 @@
         <v>16</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -952,10 +959,10 @@
         <v>17</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
@@ -975,10 +982,10 @@
         <v>18</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -998,10 +1005,10 @@
         <v>19</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -1021,10 +1028,10 @@
         <v>20</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -1044,10 +1051,10 @@
         <v>22</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>45</v>
       </c>
@@ -1067,10 +1074,10 @@
         <v>23</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1090,10 +1097,10 @@
         <v>24</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
@@ -1113,10 +1120,10 @@
         <v>25</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1136,10 +1143,10 @@
         <v>26</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1159,10 +1166,10 @@
         <v>28</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>45</v>
       </c>
@@ -1182,10 +1189,10 @@
         <v>29</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>45</v>
       </c>
@@ -1205,10 +1212,10 @@
         <v>30</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
@@ -1228,10 +1235,10 @@
         <v>31</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>45</v>
       </c>
@@ -1251,10 +1258,10 @@
         <v>32</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>45</v>
       </c>
@@ -1274,10 +1281,10 @@
         <v>34</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
@@ -1297,10 +1304,10 @@
         <v>35</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>45</v>
       </c>
@@ -1320,10 +1327,10 @@
         <v>36</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>45</v>
       </c>
@@ -1343,10 +1350,10 @@
         <v>37</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>45</v>
       </c>
@@ -1366,10 +1373,10 @@
         <v>38</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1389,10 +1396,10 @@
         <v>46</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1412,10 +1419,10 @@
         <v>47</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1435,10 +1442,10 @@
         <v>48</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1458,10 +1465,10 @@
         <v>49</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -1481,10 +1488,10 @@
         <v>50</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -1504,10 +1511,10 @@
         <v>51</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>9</v>
       </c>
@@ -1527,10 +1534,10 @@
         <v>52</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>9</v>
       </c>
@@ -1550,10 +1557,10 @@
         <v>53</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>9</v>
       </c>
@@ -1573,10 +1580,10 @@
         <v>54</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>27</v>
       </c>
@@ -1596,10 +1603,10 @@
         <v>55</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>27</v>
       </c>
@@ -1619,10 +1626,10 @@
         <v>56</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>27</v>
       </c>
@@ -1642,10 +1649,10 @@
         <v>57</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="63" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
         <v>7</v>
       </c>
@@ -1665,7 +1672,7 @@
         <v>58</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Search functionality now works when group nodes are off
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{358FA640-42BC-4F78-9FC6-7BD135EFCA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDC40CB-E1D2-4CAE-BBFB-09CD81F5A404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="4080" windowWidth="29040" windowHeight="16440" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="64">
   <si>
     <t>CI_Type</t>
   </si>
@@ -222,11 +222,16 @@
  </t>
   </si>
   <si>
-    <t xml:space="preserve">Business description…HELLO
-Attribute 1: Value
-Attribute 2: Value
-Attribute 3: Value
- </t>
+    <t>Tech 54</t>
+  </si>
+  <si>
+    <t>Data 54</t>
+  </si>
+  <si>
+    <t>Location 93</t>
+  </si>
+  <si>
+    <t>Person 93</t>
   </si>
 </sst>
 </file>
@@ -645,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G44"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.45"/>
@@ -686,7 +691,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -706,10 +711,10 @@
         <v>40</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
@@ -729,10 +734,10 @@
         <v>41</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
@@ -752,10 +757,10 @@
         <v>42</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -775,10 +780,10 @@
         <v>44</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>45</v>
       </c>
@@ -798,10 +803,10 @@
         <v>43</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
@@ -821,10 +826,10 @@
         <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
@@ -844,10 +849,10 @@
         <v>11</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>45</v>
       </c>
@@ -867,10 +872,10 @@
         <v>12</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
@@ -890,10 +895,10 @@
         <v>13</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
@@ -913,10 +918,10 @@
         <v>14</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
@@ -936,10 +941,10 @@
         <v>16</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -959,10 +964,10 @@
         <v>17</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
@@ -982,10 +987,10 @@
         <v>18</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -1005,10 +1010,10 @@
         <v>19</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -1028,10 +1033,10 @@
         <v>20</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -1051,10 +1056,10 @@
         <v>22</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>45</v>
       </c>
@@ -1074,10 +1079,10 @@
         <v>23</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1097,10 +1102,10 @@
         <v>24</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
@@ -1120,10 +1125,10 @@
         <v>25</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1143,10 +1148,10 @@
         <v>26</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1166,10 +1171,10 @@
         <v>28</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>45</v>
       </c>
@@ -1189,10 +1194,10 @@
         <v>29</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>45</v>
       </c>
@@ -1212,10 +1217,10 @@
         <v>30</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
@@ -1235,10 +1240,10 @@
         <v>31</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>45</v>
       </c>
@@ -1258,10 +1263,10 @@
         <v>32</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>45</v>
       </c>
@@ -1281,10 +1286,10 @@
         <v>34</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
@@ -1304,10 +1309,10 @@
         <v>35</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>45</v>
       </c>
@@ -1327,10 +1332,10 @@
         <v>36</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>45</v>
       </c>
@@ -1350,10 +1355,10 @@
         <v>37</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>45</v>
       </c>
@@ -1373,10 +1378,10 @@
         <v>38</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>7</v>
       </c>
@@ -1396,10 +1401,10 @@
         <v>46</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>7</v>
       </c>
@@ -1419,10 +1424,10 @@
         <v>47</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>7</v>
       </c>
@@ -1442,10 +1447,10 @@
         <v>48</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -1465,10 +1470,10 @@
         <v>49</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -1488,10 +1493,10 @@
         <v>50</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -1511,10 +1516,10 @@
         <v>51</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>9</v>
       </c>
@@ -1534,10 +1539,10 @@
         <v>52</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>9</v>
       </c>
@@ -1557,10 +1562,10 @@
         <v>53</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>9</v>
       </c>
@@ -1574,21 +1579,21 @@
         <v>8</v>
       </c>
       <c r="E40" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="63" x14ac:dyDescent="0.45">
-      <c r="A41" s="3" t="s">
-        <v>27</v>
-      </c>
       <c r="B41" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>59</v>
@@ -1600,18 +1605,18 @@
         <v>21</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>59</v>
@@ -1620,16 +1625,16 @@
         <v>8</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A43" s="3" t="s">
         <v>27</v>
       </c>
@@ -1643,21 +1648,21 @@
         <v>8</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="63" x14ac:dyDescent="0.45">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A44" s="3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>59</v>
@@ -1669,10 +1674,102 @@
         <v>15</v>
       </c>
       <c r="F44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G44" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G45" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+      <c r="A46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G46" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+      <c r="A47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
+      <c r="A48" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G44" s="4" t="s">
-        <v>60</v>
+      <c r="G48" s="4" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Group toggles display alphabetically
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4BFC87-4AE1-4791-8E55-DB4CB39936F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12F3630-448D-4DAE-A555-DC7A65D65FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="56">
   <si>
     <t>CI_Type</t>
   </si>
@@ -208,10 +208,6 @@
   </si>
   <si>
     <t xml:space="preserve">PO 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Business description...
- </t>
   </si>
 </sst>
 </file>
@@ -632,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.45"/>
@@ -671,7 +667,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
         <v>45</v>
       </c>
@@ -679,7 +675,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>8</v>
@@ -691,10 +687,10 @@
         <v>40</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
@@ -702,7 +698,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -714,10 +710,10 @@
         <v>41</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>45</v>
       </c>
@@ -725,7 +721,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
@@ -737,10 +733,10 @@
         <v>42</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
         <v>45</v>
       </c>
@@ -748,7 +744,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
@@ -760,10 +756,10 @@
         <v>44</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
         <v>45</v>
       </c>
@@ -771,7 +767,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
@@ -783,10 +779,10 @@
         <v>43</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
@@ -794,7 +790,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
@@ -806,10 +802,10 @@
         <v>10</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
@@ -817,7 +813,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
@@ -829,10 +825,10 @@
         <v>11</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
         <v>45</v>
       </c>
@@ -840,7 +836,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
@@ -852,10 +848,10 @@
         <v>12</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A10" s="3" t="s">
         <v>45</v>
       </c>
@@ -863,7 +859,7 @@
         <v>6</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>8</v>
@@ -875,10 +871,10 @@
         <v>13</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
@@ -886,7 +882,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
@@ -898,10 +894,10 @@
         <v>14</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A12" s="3" t="s">
         <v>45</v>
       </c>
@@ -909,7 +905,7 @@
         <v>6</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
@@ -921,10 +917,10 @@
         <v>16</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A13" s="3" t="s">
         <v>45</v>
       </c>
@@ -932,7 +928,7 @@
         <v>6</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
@@ -944,10 +940,10 @@
         <v>17</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
@@ -955,7 +951,7 @@
         <v>6</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
@@ -967,10 +963,10 @@
         <v>18</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>45</v>
       </c>
@@ -978,7 +974,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -990,10 +986,10 @@
         <v>19</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -1001,7 +997,7 @@
         <v>6</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -1013,10 +1009,10 @@
         <v>20</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -1024,7 +1020,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>8</v>
@@ -1036,10 +1032,10 @@
         <v>22</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>45</v>
       </c>
@@ -1047,7 +1043,7 @@
         <v>6</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>8</v>
@@ -1059,10 +1055,10 @@
         <v>23</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -1070,7 +1066,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>8</v>
@@ -1082,10 +1078,10 @@
         <v>24</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>45</v>
       </c>
@@ -1093,7 +1089,7 @@
         <v>6</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>8</v>
@@ -1105,10 +1101,10 @@
         <v>25</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1116,7 +1112,7 @@
         <v>6</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>8</v>
@@ -1128,10 +1124,10 @@
         <v>26</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1139,7 +1135,7 @@
         <v>6</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>8</v>
@@ -1151,10 +1147,10 @@
         <v>28</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>45</v>
       </c>
@@ -1162,7 +1158,7 @@
         <v>6</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>8</v>
@@ -1174,10 +1170,10 @@
         <v>29</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>45</v>
       </c>
@@ -1185,7 +1181,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>8</v>
@@ -1197,10 +1193,10 @@
         <v>30</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
@@ -1208,7 +1204,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>8</v>
@@ -1220,10 +1216,10 @@
         <v>31</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>45</v>
       </c>
@@ -1231,7 +1227,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>8</v>
@@ -1243,10 +1239,10 @@
         <v>32</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>45</v>
       </c>
@@ -1254,7 +1250,7 @@
         <v>6</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>8</v>
@@ -1266,10 +1262,10 @@
         <v>34</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
@@ -1277,7 +1273,7 @@
         <v>6</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>8</v>
@@ -1289,10 +1285,10 @@
         <v>35</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>45</v>
       </c>
@@ -1300,7 +1296,7 @@
         <v>6</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>8</v>
@@ -1312,10 +1308,10 @@
         <v>36</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>45</v>
       </c>
@@ -1323,7 +1319,7 @@
         <v>6</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>8</v>
@@ -1335,10 +1331,10 @@
         <v>37</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>45</v>
       </c>
@@ -1346,7 +1342,7 @@
         <v>6</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>8</v>
@@ -1358,10 +1354,10 @@
         <v>38</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>15</v>
       </c>
@@ -1369,7 +1365,7 @@
         <v>20</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>8</v>
@@ -1381,10 +1377,10 @@
         <v>48</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A33" s="3" t="s">
         <v>15</v>
       </c>
@@ -1392,7 +1388,7 @@
         <v>20</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>8</v>
@@ -1404,10 +1400,10 @@
         <v>49</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A34" s="3" t="s">
         <v>9</v>
       </c>
@@ -1415,7 +1411,7 @@
         <v>10</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>8</v>
@@ -1427,10 +1423,10 @@
         <v>50</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A35" s="3" t="s">
         <v>21</v>
       </c>
@@ -1438,7 +1434,7 @@
         <v>25</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>8</v>
@@ -1450,10 +1446,10 @@
         <v>46</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A36" s="3" t="s">
         <v>7</v>
       </c>
@@ -1461,7 +1457,7 @@
         <v>41</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>8</v>
@@ -1473,10 +1469,10 @@
         <v>51</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A37" s="3" t="s">
         <v>7</v>
       </c>
@@ -1484,7 +1480,7 @@
         <v>41</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>8</v>
@@ -1496,10 +1492,10 @@
         <v>52</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A38" s="3" t="s">
         <v>7</v>
       </c>
@@ -1507,7 +1503,7 @@
         <v>41</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>8</v>
@@ -1519,10 +1515,10 @@
         <v>53</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A39" s="3" t="s">
         <v>7</v>
       </c>
@@ -1530,7 +1526,7 @@
         <v>41</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>8</v>
@@ -1542,10 +1538,10 @@
         <v>54</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A40" s="3" t="s">
         <v>7</v>
       </c>
@@ -1553,7 +1549,7 @@
         <v>40</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>8</v>
@@ -1565,10 +1561,10 @@
         <v>16</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
@@ -1576,7 +1572,7 @@
         <v>40</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>8</v>
@@ -1588,10 +1584,10 @@
         <v>22</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="21" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">
       <c r="A42" s="3" t="s">
         <v>7</v>
       </c>
@@ -1599,7 +1595,7 @@
         <v>40</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>8</v>
@@ -1611,7 +1607,7 @@
         <v>10</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="52.5" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Now getting all indirect relationships in renderGraph(), still need to create links to them
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12F3630-448D-4DAE-A555-DC7A65D65FB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FBB7F1-D1D8-441C-A5D5-ACF11F19B74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{8FD27001-DFD4-4AA0-80CB-98EF0B77155D}"/>
   </bookViews>
@@ -628,7 +628,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{007A403A-755E-4165-8DDF-621577D0D37A}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Displaying indirect relationship links and asset nodes happens in place.
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Network-Diagram-App\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FF193A-F1E7-43FB-988F-37E98D9872F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{A88976E2-E33B-4602-A50D-1F086AEB321B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="4080" windowWidth="29040" windowHeight="16440" xr2:uid="{ABE0169A-B2D0-4581-9086-DD78F64B1690}"/>
   </bookViews>
   <sheets>
-    <sheet name="complete_oit_dependencies" sheetId="1" r:id="rId1"/>
+    <sheet name="network_diagram" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="76">
   <si>
     <t>CI_Type</t>
   </si>
@@ -155,11 +155,6 @@
     <t>Microsoft Enterprise Agreement</t>
   </si>
   <si>
-    <t>PO: #9829823
-Reseller: SHI
-Ammount: $300,00</t>
-  </si>
-  <si>
     <t>Tallahassee Office</t>
   </si>
   <si>
@@ -176,9 +171,6 @@
   </si>
   <si>
     <t>Miami DC</t>
-  </si>
-  <si>
-    <t>Oracle DB</t>
   </si>
   <si>
     <t>Env: Production
@@ -201,16 +193,7 @@
     <t>A tool to manage customer or internal support requests, track issue resolution, and improve service delivery through efficient ticketing and communication.</t>
   </si>
   <si>
-    <t>Employee DB</t>
-  </si>
-  <si>
     <t>Financial Transactions DB</t>
-  </si>
-  <si>
-    <t>Tickets DB</t>
-  </si>
-  <si>
-    <t>Knowledge Base/FAQ DB</t>
   </si>
   <si>
     <t xml:space="preserve">Office of Information Technology (OIT)
@@ -255,49 +238,63 @@
 Amount: $125,000</t>
   </si>
   <si>
-    <t xml:space="preserve">Cybersecurity Maintenance Agreement
-</t>
-  </si>
-  <si>
-    <t>PO: #12975
-Reseller: Palo Alto Networks
-Amount: $150,000</t>
-  </si>
-  <si>
-    <t>Microsoft 365 Licensing Agreement</t>
-  </si>
-  <si>
-    <t>PO: #12977
-Reseller: CDW
-Amount: $275,000</t>
-  </si>
-  <si>
-    <t>PO: #12978
-Reseller: Dell Technologies
-Amount: $180,000</t>
-  </si>
-  <si>
-    <t>Network Equipment Agreement</t>
-  </si>
-  <si>
-    <t>Enterprise Storage System Agreement</t>
-  </si>
-  <si>
-    <t>PO: #12978
-Reseller: Cisco Systems
-Amount: $220,000</t>
+    <t>A system to manage employee data, recruitment, payroll, and performance.</t>
+  </si>
+  <si>
+    <t>Version: 7.0
+EOL Date: 04/02/2025
+Units: 121</t>
+  </si>
+  <si>
+    <t>PO: #12980
+Reseller: vSan
+Amount: $175,000</t>
+  </si>
+  <si>
+    <t>Human Resources DB</t>
+  </si>
+  <si>
+    <t>Help Desk DB</t>
+  </si>
+  <si>
+    <t>Oracle Database</t>
+  </si>
+  <si>
+    <t>Staffing Inc.</t>
   </si>
   <si>
     <t>PO: #12973
 Reseller: SHI
-Ammount: $300,00</t>
+Amount: $300,00</t>
+  </si>
+  <si>
+    <t>PO: #9829232
+Amount: $127,500</t>
+  </si>
+  <si>
+    <t>PO: #9829823
+Reseller: SHI
+Amount: $300,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oracle </t>
+  </si>
+  <si>
+    <t>PO: #1298009
+Reseller: SHI
+Amount: $200,000</t>
+  </si>
+  <si>
+    <t>PO: #1298009
+Reseller: SHI
+Amount: $200,001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -434,8 +431,14 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -791,21 +794,23 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1186,48 +1191,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C12307-1723-46DD-B559-145BAE511595}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="21.1328125" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.73046875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="79.1328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="68.265625" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.06640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.86328125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="1"/>
+    <col min="7" max="7" width="57.53125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="23.73046875" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" ht="57" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1235,7 +1241,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -1247,7 +1253,7 @@
         <v>32</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
@@ -1258,7 +1264,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>
@@ -1270,10 +1276,10 @@
         <v>33</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1281,7 +1287,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>9</v>
@@ -1292,11 +1298,11 @@
       <c r="F4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="G4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -1304,7 +1310,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>9</v>
@@ -1315,11 +1321,11 @@
       <c r="F5" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="G5" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1327,7 +1333,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
@@ -1338,11 +1344,11 @@
       <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="G6" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1350,22 +1356,22 @@
         <v>8</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1373,22 +1379,22 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1396,22 +1402,22 @@
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1419,22 +1425,22 @@
         <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -1442,19 +1448,19 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1465,19 +1471,19 @@
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>63</v>
+        <v>12</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1488,19 +1494,19 @@
         <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1511,19 +1517,19 @@
         <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1534,19 +1540,19 @@
         <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1557,19 +1563,19 @@
         <v>8</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1580,19 +1586,19 @@
         <v>8</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1603,19 +1609,19 @@
         <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1626,19 +1632,19 @@
         <v>8</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>56</v>
+        <v>17</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1649,19 +1655,19 @@
         <v>8</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1672,19 +1678,19 @@
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>58</v>
+        <v>17</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1695,19 +1701,19 @@
         <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1718,280 +1724,283 @@
         <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
-        <v>7</v>
+      <c r="A25" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B27" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>73</v>
+        <v>17</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A32" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A33" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A34" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G28" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G30" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F32" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G32" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A33" s="1" t="s">
+      <c r="D34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="F34" s="1" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A35" s="1" t="s">
-        <v>10</v>
+      <c r="A35" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>9</v>
@@ -2000,67 +2009,67 @@
         <v>17</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>9</v>
@@ -2069,56 +2078,56 @@
         <v>20</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="F39" s="1" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="F40" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2135,13 +2144,13 @@
         <v>9</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2158,82 +2167,112 @@
         <v>9</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E44" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A46" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="B45" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>22</v>
+      <c r="B46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G44">
+    <sortCondition ref="A2:A44" customList="Organization"/>
+  </sortState>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
See All Assets functionality
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6BCFD1-BD47-4760-9B5E-E40000629C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2A0B3C-9BCC-4B47-8E2A-BDC2819737CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="4080" windowWidth="29040" windowHeight="16440" xr2:uid="{ABE0169A-B2D0-4581-9086-DD78F64B1690}"/>
+    <workbookView xWindow="-38520" yWindow="3510" windowWidth="38640" windowHeight="21840" xr2:uid="{ABE0169A-B2D0-4581-9086-DD78F64B1690}"/>
   </bookViews>
   <sheets>
     <sheet name="network_diagram" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="82">
   <si>
     <t>CI_Type</t>
   </si>
@@ -284,11 +284,6 @@
     <t>Corporate headquarters.</t>
   </si>
   <si>
-    <t>POS #: Staff Aug
-Title: Oracle DB Admin - Lead
-S+B: $130,750</t>
-  </si>
-  <si>
     <t>POS #: 345234
 Title:  Business Analyst
 S+B: $130,750</t>
@@ -315,6 +310,11 @@
     <t>Env: Production
 Type: Oracle Server
 Size: 46.5 GB</t>
+  </si>
+  <si>
+    <t>POS #: Staff Aug
+Title:  DB Admin - Lead
+S+B: $130,750</t>
   </si>
 </sst>
 </file>
@@ -1284,11 +1284,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C12307-1723-46DD-B559-145BAE511595}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1577,7 +1577,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1600,7 +1600,7 @@
         <v>16</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1623,7 +1623,7 @@
         <v>13</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1646,7 +1646,7 @@
         <v>12</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1669,7 +1669,7 @@
         <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -1712,7 +1712,7 @@
         <v>20</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>64</v>
@@ -2037,7 +2037,7 @@
         <v>16</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2060,7 +2060,7 @@
         <v>15</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2083,7 +2083,7 @@
         <v>15</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2106,7 +2106,7 @@
         <v>13</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -2129,7 +2129,7 @@
         <v>13</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2225,14 +2225,14 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A41" s="8" t="s">
-        <v>10</v>
+      <c r="A41" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>9</v>
@@ -2241,21 +2241,21 @@
         <v>17</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>9</v>
@@ -2264,21 +2264,21 @@
         <v>17</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>9</v>
@@ -2287,10 +2287,10 @@
         <v>17</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2298,10 +2298,10 @@
         <v>19</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>9</v>
@@ -2310,21 +2310,21 @@
         <v>17</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>9</v>
@@ -2340,26 +2340,26 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A46" s="4" t="s">
-        <v>19</v>
+      <c r="A46" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="7" t="s">
-        <v>17</v>
+      <c r="E46" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2367,7 +2367,7 @@
         <v>11</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>76</v>
@@ -2390,7 +2390,7 @@
         <v>11</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>77</v>
@@ -2413,7 +2413,7 @@
         <v>11</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>78</v>
@@ -2436,10 +2436,10 @@
         <v>11</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>9</v>
@@ -2459,22 +2459,22 @@
         <v>11</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E51" s="10" t="s">
-        <v>21</v>
+      <c r="E51" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2482,10 +2482,10 @@
         <v>11</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>9</v>
@@ -2497,30 +2497,30 @@
         <v>61</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="G53" s="1" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2528,10 +2528,10 @@
         <v>17</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>9</v>
@@ -2543,7 +2543,7 @@
         <v>14</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2551,22 +2551,22 @@
         <v>17</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="12" t="s">
+      <c r="E55" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2574,10 +2574,10 @@
         <v>17</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>9</v>
@@ -2589,7 +2589,7 @@
         <v>12</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2597,10 +2597,10 @@
         <v>17</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>9</v>
@@ -2612,7 +2612,7 @@
         <v>12</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2620,22 +2620,22 @@
         <v>17</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="6" t="s">
-        <v>11</v>
+      <c r="E58" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2643,10 +2643,10 @@
         <v>17</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>9</v>
@@ -2666,10 +2666,10 @@
         <v>17</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>9</v>
@@ -2678,10 +2678,10 @@
         <v>20</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>36</v>
+        <v>79</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2689,10 +2689,10 @@
         <v>17</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>9</v>
@@ -2701,10 +2701,10 @@
         <v>20</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
@@ -2712,10 +2712,10 @@
         <v>17</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>9</v>
@@ -2724,41 +2724,18 @@
         <v>20</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A63" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G63" s="1" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J70">
-    <sortCondition ref="A2:A70" customList="Organization"/>
-    <sortCondition ref="E2:E70"/>
-    <sortCondition ref="B2:B70"/>
-    <sortCondition ref="F2:F70"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J69">
+    <sortCondition ref="A2:A69" customList="Organization"/>
+    <sortCondition ref="E2:E69"/>
+    <sortCondition ref="B2:B69"/>
+    <sortCondition ref="F2:F69"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
search functionality searches all assets
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9AA4BA-4C92-4094-A144-3F173210233E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B15FD45-DFCD-4DE9-B4BB-97783305A5CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="3510" windowWidth="38640" windowHeight="21840" xr2:uid="{ABE0169A-B2D0-4581-9086-DD78F64B1690}"/>
   </bookViews>
@@ -471,7 +471,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -696,6 +696,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -860,7 +866,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -899,6 +905,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1284,11 +1293,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C12307-1723-46DD-B559-145BAE511595}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63:D87"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2730,6 +2739,7 @@
         <v>57</v>
       </c>
     </row>
+    <row r="63" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J69">
     <sortCondition ref="A2:A69" customList="Organization"/>

</xml_diff>

<commit_message>
right container assets stay the same.
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691971FF-5016-4742-A25F-276C164BFE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729DA74D-073C-4618-BB59-A0AF603581CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{ABE0169A-B2D0-4581-9086-DD78F64B1690}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="82">
   <si>
     <t>CI_Type</t>
   </si>
@@ -315,150 +315,6 @@
     <t>POS #: Staff Aug
 Title:  DB Admin - Lead
 S+B: $130,750</t>
-  </si>
-  <si>
-    <t>Michael Johnson</t>
-  </si>
-  <si>
-    <t>Emily Davis</t>
-  </si>
-  <si>
-    <t>Robert Brown</t>
-  </si>
-  <si>
-    <t>Linda Wilson</t>
-  </si>
-  <si>
-    <t>William Martinez</t>
-  </si>
-  <si>
-    <t>Elizabeth Anderson</t>
-  </si>
-  <si>
-    <t>David Thomas</t>
-  </si>
-  <si>
-    <t>Susan Taylor</t>
-  </si>
-  <si>
-    <t>James White</t>
-  </si>
-  <si>
-    <t>Patricia Harris</t>
-  </si>
-  <si>
-    <t>Christopher Martin</t>
-  </si>
-  <si>
-    <t>Jessica Thompson</t>
-  </si>
-  <si>
-    <t>Daniel Garcia</t>
-  </si>
-  <si>
-    <t>Sarah Robinson</t>
-  </si>
-  <si>
-    <t>Matthew Clark</t>
-  </si>
-  <si>
-    <t>Ashley Rodriguez</t>
-  </si>
-  <si>
-    <t>Joshua Lewis</t>
-  </si>
-  <si>
-    <t>Megan Lee</t>
-  </si>
-  <si>
-    <t>Andrew Walker</t>
-  </si>
-  <si>
-    <t>Stephanie Hall</t>
-  </si>
-  <si>
-    <t>Joseph Allen</t>
-  </si>
-  <si>
-    <t>Rebecca Young</t>
-  </si>
-  <si>
-    <t>Kevin King</t>
-  </si>
-  <si>
-    <t>Laura Wright</t>
-  </si>
-  <si>
-    <t>Brian Scott</t>
-  </si>
-  <si>
-    <t>Olivia Green</t>
-  </si>
-  <si>
-    <t>Ryan Adams</t>
-  </si>
-  <si>
-    <t>Sophia Baker</t>
-  </si>
-  <si>
-    <t>Brandon Nelson</t>
-  </si>
-  <si>
-    <t>Isabella Carter</t>
-  </si>
-  <si>
-    <t>Justin Mitchell</t>
-  </si>
-  <si>
-    <t>Emma Perez</t>
-  </si>
-  <si>
-    <t>Samuel Roberts</t>
-  </si>
-  <si>
-    <t>Hannah Phillips</t>
-  </si>
-  <si>
-    <t>Jason Evans</t>
-  </si>
-  <si>
-    <t>Madison Campbell</t>
-  </si>
-  <si>
-    <t>Ethan Parker</t>
-  </si>
-  <si>
-    <t>Abigail Murphy</t>
-  </si>
-  <si>
-    <t>Alexander Edwards</t>
-  </si>
-  <si>
-    <t>Charlotte Ward</t>
-  </si>
-  <si>
-    <t>Jacob Hughes</t>
-  </si>
-  <si>
-    <t>Amelia Peterson</t>
-  </si>
-  <si>
-    <t>Nicholas Flores</t>
-  </si>
-  <si>
-    <t>Ava Rivera</t>
-  </si>
-  <si>
-    <t>Jonathan Morris</t>
-  </si>
-  <si>
-    <t>Chloe Cooper</t>
-  </si>
-  <si>
-    <t>Benjamin Reed</t>
-  </si>
-  <si>
-    <t>Lily Bailey</t>
   </si>
 </sst>
 </file>
@@ -1437,11 +1293,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C12307-1723-46DD-B559-145BAE511595}">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F114" sqref="F114"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63:D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2883,1156 +2739,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="14" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A63" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A64" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E64" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G64" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A65" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A66" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A67" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F67" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A68" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E68" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A69" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A70" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A71" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A72" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A73" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="G73" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A74" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E74" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G74" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A75" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A76" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A77" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A78" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E78" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A79" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E79" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A80" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E80" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G80" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A81" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G81" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A82" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A83" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E83" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A84" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B84" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E84" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A85" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A86" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A87" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A88" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E88" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A89" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B89" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E89" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A90" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B90" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A91" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A92" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B92" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E92" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G92" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A93" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B93" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E93" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A94" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E94" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G94" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A95" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E95" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G95" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A96" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E96" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F96" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G96" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A97" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E97" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G97" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A98" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B98" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E98" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F98" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="G98" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A99" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B99" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E99" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F99" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A100" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B100" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D100" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E100" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F100" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A101" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B101" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E101" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F101" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A102" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B102" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C102" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D102" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E102" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="G102" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A103" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D103" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E103" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F103" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G103" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A104" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B104" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D104" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E104" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F104" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G104" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A105" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B105" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C105" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E105" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="G105" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A106" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B106" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C106" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D106" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E106" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F106" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G106" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A107" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B107" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C107" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D107" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E107" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F107" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G107" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A108" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B108" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C108" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D108" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E108" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F108" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G108" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A109" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B109" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C109" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D109" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E109" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F109" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G109" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A110" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C110" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E110" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F110" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G110" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A111" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B111" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C111" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D111" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E111" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F111" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A112" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B112" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C112" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D112" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E112" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F112" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="G112" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
+    <row r="63" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J69">
     <sortCondition ref="A2:A69" customList="Organization"/>

</xml_diff>

<commit_message>
*** all data on right side is loaded in right container and never changed ***
</commit_message>
<xml_diff>
--- a/data/network_diagram.xlsx
+++ b/data/network_diagram.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaden Humphries\Desktop\Scott's Diagram\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729DA74D-073C-4618-BB59-A0AF603581CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C15CFC26-4D8E-4144-BE29-1750C4A9D063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{ABE0169A-B2D0-4581-9086-DD78F64B1690}"/>
+    <workbookView xWindow="-38520" yWindow="1140" windowWidth="38640" windowHeight="21840" xr2:uid="{ABE0169A-B2D0-4581-9086-DD78F64B1690}"/>
   </bookViews>
   <sheets>
     <sheet name="network_diagram" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="91">
   <si>
     <t>CI_Type</t>
   </si>
@@ -315,6 +315,41 @@
     <t>POS #: Staff Aug
 Title:  DB Admin - Lead
 S+B: $130,750</t>
+  </si>
+  <si>
+    <t>Liam Anderson</t>
+  </si>
+  <si>
+    <t>Emma Roberts</t>
+  </si>
+  <si>
+    <t>Noah Carter</t>
+  </si>
+  <si>
+    <t>Olivia Mitchell</t>
+  </si>
+  <si>
+    <t>William Turner</t>
+  </si>
+  <si>
+    <t>POS #: Staff Aug
+Title:  DB Admin - Lead
+S+B: $130,751</t>
+  </si>
+  <si>
+    <t>POS #: Staff Aug
+Title:  DB Admin - Lead
+S+B: $130,752</t>
+  </si>
+  <si>
+    <t>POS #: Staff Aug
+Title:  DB Admin - Lead
+S+B: $130,753</t>
+  </si>
+  <si>
+    <t>POS #: Staff Aug
+Title:  DB Admin - Lead
+S+B: $130,754</t>
   </si>
 </sst>
 </file>
@@ -1293,11 +1328,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48C12307-1723-46DD-B559-145BAE511595}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63:D88"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2739,7 +2774,201 @@
         <v>57</v>
       </c>
     </row>
-    <row r="63" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="63" spans="1:7" s="14" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A63" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A64" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A65" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A66" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A67" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A68" s="3"/>
+      <c r="E68" s="6"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A69" s="3"/>
+      <c r="E69" s="6"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A70" s="3"/>
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A71" s="3"/>
+      <c r="E71" s="6"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A72" s="3"/>
+      <c r="E72" s="6"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A73" s="3"/>
+      <c r="E73" s="6"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A74" s="3"/>
+      <c r="E74" s="6"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A75" s="3"/>
+      <c r="E75" s="6"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A76" s="3"/>
+      <c r="E76" s="6"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A77" s="3"/>
+      <c r="E77" s="6"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A78" s="3"/>
+      <c r="E78" s="6"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A79" s="3"/>
+      <c r="E79" s="6"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A80" s="3"/>
+      <c r="E80" s="6"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A81" s="3"/>
+      <c r="E81" s="6"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A82" s="3"/>
+      <c r="E82" s="6"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A83" s="3"/>
+      <c r="E83" s="6"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A84" s="3"/>
+      <c r="E84" s="6"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A85" s="3"/>
+      <c r="E85" s="6"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A86" s="3"/>
+      <c r="E86" s="6"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A87" s="3"/>
+      <c r="E87" s="6"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J69">
     <sortCondition ref="A2:A69" customList="Organization"/>

</xml_diff>